<commit_message>
added release table and some updated data
</commit_message>
<xml_diff>
--- a/data_raw/smelt/abundance_estimates.xlsx
+++ b/data_raw/smelt/abundance_estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/samt_smt_assessments/data_raw/smelt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3030992D-F2E3-4C0A-A39D-38395044D36B}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07857C59-C7E7-45A7-AA3A-0A60F38D89D1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1080" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="42">
   <si>
     <t>Week</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>October 6–10, 2025</t>
+  </si>
+  <si>
+    <t>October 13–17, 2025</t>
+  </si>
+  <si>
+    <t>October 20–24, 2025</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6CDBE-81F8-437E-8236-059C4BBF9395}">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection sqref="A1:K143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1138,7 @@
         <v>94</v>
       </c>
       <c r="K17" s="1">
-        <v>3491</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1307,7 +1313,7 @@
         <v>94</v>
       </c>
       <c r="K22" s="1">
-        <v>3491</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2106,13 +2112,13 @@
         <v>113446</v>
       </c>
       <c r="I45">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="J45">
         <v>83</v>
       </c>
       <c r="K45" s="1">
-        <v>3297</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2281,13 +2287,13 @@
         <v>485151</v>
       </c>
       <c r="I50">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="J50">
         <v>83</v>
       </c>
       <c r="K50" s="1">
-        <v>3297</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3576,13 +3582,13 @@
         <v>98810</v>
       </c>
       <c r="I87">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J87">
         <v>78</v>
       </c>
       <c r="K87" s="1">
-        <v>3309</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -3751,13 +3757,13 @@
         <v>532159</v>
       </c>
       <c r="I92">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J92">
         <v>78</v>
       </c>
       <c r="K92" s="1">
-        <v>3309</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -4871,13 +4877,13 @@
         <v>113833</v>
       </c>
       <c r="I124">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J124">
         <v>78</v>
       </c>
       <c r="K124" s="1">
-        <v>3119</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
@@ -4906,13 +4912,13 @@
         <v>97872</v>
       </c>
       <c r="I125">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J125">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K125" s="1">
-        <v>1602</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -4938,7 +4944,7 @@
         <v>0</v>
       </c>
       <c r="H126" s="1">
-        <v>70930</v>
+        <v>70931</v>
       </c>
       <c r="I126" t="s">
         <v>12</v>
@@ -4973,7 +4979,7 @@
         <v>0</v>
       </c>
       <c r="H127" s="1">
-        <v>84687</v>
+        <v>84693</v>
       </c>
       <c r="I127" t="s">
         <v>12</v>
@@ -5043,16 +5049,506 @@
         <v>0</v>
       </c>
       <c r="H129" s="1">
-        <v>546420</v>
+        <v>546427</v>
       </c>
       <c r="I129" s="1">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J129">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K129" s="1">
-        <v>3866</v>
+        <v>3859</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>20</v>
+      </c>
+      <c r="B130" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130">
+        <v>6</v>
+      </c>
+      <c r="D130">
+        <v>24</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130" s="1">
+        <v>115859</v>
+      </c>
+      <c r="I130" t="s">
+        <v>12</v>
+      </c>
+      <c r="J130" t="s">
+        <v>13</v>
+      </c>
+      <c r="K130" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>20</v>
+      </c>
+      <c r="B131" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+      <c r="D131">
+        <v>22</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131" s="1">
+        <v>102403</v>
+      </c>
+      <c r="I131">
+        <v>817</v>
+      </c>
+      <c r="J131">
+        <v>82</v>
+      </c>
+      <c r="K131" s="1">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>20</v>
+      </c>
+      <c r="B132" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132">
+        <v>6</v>
+      </c>
+      <c r="D132">
+        <v>24</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132" s="1">
+        <v>94714</v>
+      </c>
+      <c r="I132" t="s">
+        <v>12</v>
+      </c>
+      <c r="J132" t="s">
+        <v>13</v>
+      </c>
+      <c r="K132" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>20</v>
+      </c>
+      <c r="B133" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133">
+        <v>6</v>
+      </c>
+      <c r="D133">
+        <v>23</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133" s="1">
+        <v>84701</v>
+      </c>
+      <c r="I133" t="s">
+        <v>12</v>
+      </c>
+      <c r="J133" t="s">
+        <v>13</v>
+      </c>
+      <c r="K133" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>20</v>
+      </c>
+      <c r="B134" t="s">
+        <v>17</v>
+      </c>
+      <c r="C134">
+        <v>5</v>
+      </c>
+      <c r="D134">
+        <v>20</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="H134" s="1">
+        <v>72976</v>
+      </c>
+      <c r="I134" t="s">
+        <v>12</v>
+      </c>
+      <c r="J134" t="s">
+        <v>13</v>
+      </c>
+      <c r="K134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>20</v>
+      </c>
+      <c r="B135" t="s">
+        <v>18</v>
+      </c>
+      <c r="C135">
+        <v>6</v>
+      </c>
+      <c r="D135">
+        <v>24</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135" s="1">
+        <v>95140</v>
+      </c>
+      <c r="I135" t="s">
+        <v>12</v>
+      </c>
+      <c r="J135" t="s">
+        <v>13</v>
+      </c>
+      <c r="K135" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>20</v>
+      </c>
+      <c r="B136" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136">
+        <v>35</v>
+      </c>
+      <c r="D136">
+        <v>137</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="H136" s="1">
+        <v>565794</v>
+      </c>
+      <c r="I136">
+        <v>817</v>
+      </c>
+      <c r="J136">
+        <v>82</v>
+      </c>
+      <c r="K136" s="1">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>21</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137">
+        <v>6</v>
+      </c>
+      <c r="D137">
+        <v>24</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="H137" s="1">
+        <v>111321</v>
+      </c>
+      <c r="I137" t="s">
+        <v>12</v>
+      </c>
+      <c r="J137" t="s">
+        <v>13</v>
+      </c>
+      <c r="K137" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>21</v>
+      </c>
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138">
+        <v>6</v>
+      </c>
+      <c r="D138">
+        <v>22</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138" s="1">
+        <v>115261</v>
+      </c>
+      <c r="I138" t="s">
+        <v>12</v>
+      </c>
+      <c r="J138" t="s">
+        <v>13</v>
+      </c>
+      <c r="K138" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>21</v>
+      </c>
+      <c r="B139" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139">
+        <v>5</v>
+      </c>
+      <c r="D139">
+        <v>19</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139" s="1">
+        <v>77035</v>
+      </c>
+      <c r="I139" t="s">
+        <v>12</v>
+      </c>
+      <c r="J139" t="s">
+        <v>13</v>
+      </c>
+      <c r="K139" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>21</v>
+      </c>
+      <c r="B140" t="s">
+        <v>16</v>
+      </c>
+      <c r="C140">
+        <v>6</v>
+      </c>
+      <c r="D140">
+        <v>22</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140" s="1">
+        <v>71683</v>
+      </c>
+      <c r="I140" t="s">
+        <v>12</v>
+      </c>
+      <c r="J140" t="s">
+        <v>13</v>
+      </c>
+      <c r="K140" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>21</v>
+      </c>
+      <c r="B141" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141">
+        <v>6</v>
+      </c>
+      <c r="D141">
+        <v>24</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141" s="1">
+        <v>92880</v>
+      </c>
+      <c r="I141" t="s">
+        <v>12</v>
+      </c>
+      <c r="J141" t="s">
+        <v>13</v>
+      </c>
+      <c r="K141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>21</v>
+      </c>
+      <c r="B142" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142">
+        <v>6</v>
+      </c>
+      <c r="D142">
+        <v>24</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142" s="1">
+        <v>94594</v>
+      </c>
+      <c r="I142" t="s">
+        <v>12</v>
+      </c>
+      <c r="J142" t="s">
+        <v>13</v>
+      </c>
+      <c r="K142" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>21</v>
+      </c>
+      <c r="B143" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143">
+        <v>35</v>
+      </c>
+      <c r="D143">
+        <v>135</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143" s="1">
+        <v>562775</v>
+      </c>
+      <c r="I143" t="s">
+        <v>12</v>
+      </c>
+      <c r="J143" t="s">
+        <v>13</v>
+      </c>
+      <c r="K143" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -5062,10 +5558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5A6928-3806-4082-94AB-A52936AB7317}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5234,6 +5730,22 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
abundance estimate data update
</commit_message>
<xml_diff>
--- a/data_raw/smelt/abundance_estimates.xlsx
+++ b/data_raw/smelt/abundance_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/samt_smt_assessments/data_raw/smelt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07857C59-C7E7-45A7-AA3A-0A60F38D89D1}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{369A288A-4D36-465C-A6B8-A3EF8A13BCA2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
+    <workbookView xWindow="-27375" yWindow="3285" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="43">
   <si>
     <t>Week</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>October 20–24, 2025</t>
+  </si>
+  <si>
+    <t>October 27–31, 2025</t>
   </si>
 </sst>
 </file>
@@ -535,15 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6CDBE-81F8-437E-8236-059C4BBF9395}">
-  <dimension ref="A1:K143"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection sqref="A1:K143"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="L140" sqref="L140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -5548,6 +5552,251 @@
         <v>13</v>
       </c>
       <c r="K143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>22</v>
+      </c>
+      <c r="B144" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144">
+        <v>6</v>
+      </c>
+      <c r="D144">
+        <v>24</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144" s="1">
+        <v>93861</v>
+      </c>
+      <c r="I144" t="s">
+        <v>12</v>
+      </c>
+      <c r="J144" t="s">
+        <v>13</v>
+      </c>
+      <c r="K144" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>22</v>
+      </c>
+      <c r="B145" t="s">
+        <v>14</v>
+      </c>
+      <c r="C145">
+        <v>6</v>
+      </c>
+      <c r="D145">
+        <v>24</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145" s="1">
+        <v>95286</v>
+      </c>
+      <c r="I145" t="s">
+        <v>12</v>
+      </c>
+      <c r="J145" t="s">
+        <v>13</v>
+      </c>
+      <c r="K145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>22</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146">
+        <v>6</v>
+      </c>
+      <c r="D146">
+        <v>24</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146" s="1">
+        <v>94751</v>
+      </c>
+      <c r="I146" t="s">
+        <v>12</v>
+      </c>
+      <c r="J146" t="s">
+        <v>13</v>
+      </c>
+      <c r="K146" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>22</v>
+      </c>
+      <c r="B147" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147">
+        <v>6</v>
+      </c>
+      <c r="D147">
+        <v>24</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147" s="1">
+        <v>80263</v>
+      </c>
+      <c r="I147" t="s">
+        <v>12</v>
+      </c>
+      <c r="J147" t="s">
+        <v>13</v>
+      </c>
+      <c r="K147" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>22</v>
+      </c>
+      <c r="B148" t="s">
+        <v>17</v>
+      </c>
+      <c r="C148">
+        <v>6</v>
+      </c>
+      <c r="D148">
+        <v>24</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148" s="1">
+        <v>80985</v>
+      </c>
+      <c r="I148" t="s">
+        <v>12</v>
+      </c>
+      <c r="J148" t="s">
+        <v>13</v>
+      </c>
+      <c r="K148" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>22</v>
+      </c>
+      <c r="B149" t="s">
+        <v>18</v>
+      </c>
+      <c r="C149">
+        <v>6</v>
+      </c>
+      <c r="D149">
+        <v>24</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149" s="1">
+        <v>92989</v>
+      </c>
+      <c r="I149" t="s">
+        <v>12</v>
+      </c>
+      <c r="J149" t="s">
+        <v>13</v>
+      </c>
+      <c r="K149" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>22</v>
+      </c>
+      <c r="B150" t="s">
+        <v>19</v>
+      </c>
+      <c r="C150">
+        <v>36</v>
+      </c>
+      <c r="D150">
+        <v>144</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150" s="1">
+        <v>538136</v>
+      </c>
+      <c r="I150" t="s">
+        <v>12</v>
+      </c>
+      <c r="J150" t="s">
+        <v>13</v>
+      </c>
+      <c r="K150" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5558,10 +5807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5A6928-3806-4082-94AB-A52936AB7317}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5746,6 +5995,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
most recent smelt data
</commit_message>
<xml_diff>
--- a/data_raw/smelt/abundance_estimates.xlsx
+++ b/data_raw/smelt/abundance_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/samt_smt_assessments/data_raw/smelt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{369A288A-4D36-465C-A6B8-A3EF8A13BCA2}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A33791D-BB1B-44B6-8BC7-D9A42DFE0FD7}"/>
   <bookViews>
-    <workbookView xWindow="-27375" yWindow="3285" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="44">
   <si>
     <t>Week</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>October 27–31, 2025</t>
+  </si>
+  <si>
+    <t>November 3–7, 2025</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6CDBE-81F8-437E-8236-059C4BBF9395}">
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="L140" sqref="L140"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5800,6 +5803,251 @@
         <v>13</v>
       </c>
     </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>23</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+      <c r="D151">
+        <v>12</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151" s="1">
+        <v>50456</v>
+      </c>
+      <c r="I151" t="s">
+        <v>12</v>
+      </c>
+      <c r="J151" t="s">
+        <v>13</v>
+      </c>
+      <c r="K151" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>23</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152">
+        <v>6</v>
+      </c>
+      <c r="D152">
+        <v>20</v>
+      </c>
+      <c r="E152">
+        <v>19</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152" s="1">
+        <v>89408</v>
+      </c>
+      <c r="I152" s="1">
+        <v>7125</v>
+      </c>
+      <c r="J152" s="1">
+        <v>1518</v>
+      </c>
+      <c r="K152" s="1">
+        <v>21253</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>23</v>
+      </c>
+      <c r="B153" t="s">
+        <v>15</v>
+      </c>
+      <c r="C153">
+        <v>6</v>
+      </c>
+      <c r="D153">
+        <v>24</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153" s="1">
+        <v>93981</v>
+      </c>
+      <c r="I153" t="s">
+        <v>12</v>
+      </c>
+      <c r="J153" t="s">
+        <v>13</v>
+      </c>
+      <c r="K153" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>23</v>
+      </c>
+      <c r="B154" t="s">
+        <v>16</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154">
+        <v>12</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154" s="1">
+        <v>40273</v>
+      </c>
+      <c r="I154" t="s">
+        <v>12</v>
+      </c>
+      <c r="J154" t="s">
+        <v>13</v>
+      </c>
+      <c r="K154" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>23</v>
+      </c>
+      <c r="B155" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155">
+        <v>6</v>
+      </c>
+      <c r="D155">
+        <v>24</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155" s="1">
+        <v>87009</v>
+      </c>
+      <c r="I155" t="s">
+        <v>12</v>
+      </c>
+      <c r="J155" t="s">
+        <v>13</v>
+      </c>
+      <c r="K155" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>23</v>
+      </c>
+      <c r="B156" t="s">
+        <v>18</v>
+      </c>
+      <c r="C156">
+        <v>6</v>
+      </c>
+      <c r="D156">
+        <v>24</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156" s="1">
+        <v>91437</v>
+      </c>
+      <c r="I156" t="s">
+        <v>12</v>
+      </c>
+      <c r="J156" t="s">
+        <v>13</v>
+      </c>
+      <c r="K156" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>23</v>
+      </c>
+      <c r="B157" t="s">
+        <v>19</v>
+      </c>
+      <c r="C157">
+        <v>30</v>
+      </c>
+      <c r="D157">
+        <v>116</v>
+      </c>
+      <c r="E157">
+        <v>19</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157" s="1">
+        <v>452563</v>
+      </c>
+      <c r="I157" s="1">
+        <v>7125</v>
+      </c>
+      <c r="J157" s="1">
+        <v>1518</v>
+      </c>
+      <c r="K157" s="1">
+        <v>21253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5807,10 +6055,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5A6928-3806-4082-94AB-A52936AB7317}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6003,6 +6251,14 @@
         <v>42</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added and updated smelt files
</commit_message>
<xml_diff>
--- a/data_raw/smelt/abundance_estimates.xlsx
+++ b/data_raw/smelt/abundance_estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/samt_smt_assessments/data_raw/smelt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A33791D-BB1B-44B6-8BC7-D9A42DFE0FD7}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{BF3B047A-36C0-4AD4-A0BA-7FD3D60567F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35FB7A12-4F86-463A-AE32-53D466ECC9BB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
+    <workbookView xWindow="-24240" yWindow="2415" windowWidth="21600" windowHeight="12645" xr2:uid="{03E7A685-4EE0-4A4E-B4B4-B1F660F8462C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="45">
   <si>
     <t>Week</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>November 3–7, 2025</t>
+  </si>
+  <si>
+    <t>November 10–14, 2025</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6CDBE-81F8-437E-8236-059C4BBF9395}">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="F140" sqref="F140"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6048,17 +6051,263 @@
         <v>21253</v>
       </c>
     </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>24</v>
+      </c>
+      <c r="B158" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158">
+        <v>6</v>
+      </c>
+      <c r="D158">
+        <v>24</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158" s="1">
+        <v>105412</v>
+      </c>
+      <c r="I158" t="s">
+        <v>12</v>
+      </c>
+      <c r="J158" t="s">
+        <v>13</v>
+      </c>
+      <c r="K158" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>24</v>
+      </c>
+      <c r="B159" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+      <c r="D159">
+        <v>16</v>
+      </c>
+      <c r="E159">
+        <v>5</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>2</v>
+      </c>
+      <c r="H159" s="1">
+        <v>66643</v>
+      </c>
+      <c r="I159" s="1">
+        <v>3371</v>
+      </c>
+      <c r="J159">
+        <v>506</v>
+      </c>
+      <c r="K159" s="1">
+        <v>11786</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>24</v>
+      </c>
+      <c r="B160" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160">
+        <v>6</v>
+      </c>
+      <c r="D160">
+        <v>24</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160" s="1">
+        <v>94953</v>
+      </c>
+      <c r="I160" t="s">
+        <v>12</v>
+      </c>
+      <c r="J160" t="s">
+        <v>13</v>
+      </c>
+      <c r="K160" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>24</v>
+      </c>
+      <c r="B161" t="s">
+        <v>16</v>
+      </c>
+      <c r="C161">
+        <v>3</v>
+      </c>
+      <c r="D161">
+        <v>12</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161" s="1">
+        <v>36871</v>
+      </c>
+      <c r="I161" t="s">
+        <v>12</v>
+      </c>
+      <c r="J161" t="s">
+        <v>13</v>
+      </c>
+      <c r="K161" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>24</v>
+      </c>
+      <c r="B162" t="s">
+        <v>17</v>
+      </c>
+      <c r="C162">
+        <v>6</v>
+      </c>
+      <c r="D162">
+        <v>24</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162" s="1">
+        <v>73983</v>
+      </c>
+      <c r="I162" t="s">
+        <v>12</v>
+      </c>
+      <c r="J162" t="s">
+        <v>13</v>
+      </c>
+      <c r="K162" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>24</v>
+      </c>
+      <c r="B163" t="s">
+        <v>18</v>
+      </c>
+      <c r="C163">
+        <v>4</v>
+      </c>
+      <c r="D163">
+        <v>14</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163" s="1">
+        <v>60361</v>
+      </c>
+      <c r="I163" t="s">
+        <v>12</v>
+      </c>
+      <c r="J163" t="s">
+        <v>13</v>
+      </c>
+      <c r="K163" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>24</v>
+      </c>
+      <c r="B164" t="s">
+        <v>19</v>
+      </c>
+      <c r="C164">
+        <v>30</v>
+      </c>
+      <c r="D164">
+        <v>114</v>
+      </c>
+      <c r="E164">
+        <v>5</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="G164">
+        <v>2</v>
+      </c>
+      <c r="H164" s="1">
+        <v>438224</v>
+      </c>
+      <c r="I164" s="1">
+        <v>3371</v>
+      </c>
+      <c r="J164">
+        <v>506</v>
+      </c>
+      <c r="K164" s="1">
+        <v>11786</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5A6928-3806-4082-94AB-A52936AB7317}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F21"/>
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6259,6 +6508,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>